<commit_message>
add animation for chatbot, make new error log for windows error
</commit_message>
<xml_diff>
--- a/logsearch/data/error_logs/UC1_UC1_新人_11.xlsx
+++ b/logsearch/data/error_logs/UC1_UC1_新人_11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\demo-react\ntt-demo\ntt-backend\logsearch\data\error_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB419B9-287F-46C9-B865-0551B39B67C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AE1E50-78C7-4B64-9A0E-0B1E1575F044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="47">
   <si>
     <t>time</t>
   </si>
@@ -101,60 +101,10 @@
     <t>error</t>
   </si>
   <si>
-    <t>bdot20240415_141953/0415_141958_0.png</t>
-  </si>
-  <si>
-    <t>bdot20240415_141953/0415_142001_0.png</t>
-  </si>
-  <si>
-    <t>「スタート」ボタンをクリックするか、キーボードの「Windowsキー」を押す</t>
-  </si>
-  <si>
-    <t>メニューから「設定」アイコン（歯車アイコン）をクリックする</t>
-  </si>
-  <si>
-    <t>「更新とセキュリティ」オプションを選択する</t>
-  </si>
-  <si>
-    <t>左側のメニューから「Windows Update」をクリックし、Windows Update画面に移動する</t>
-  </si>
-  <si>
     <t>Error W</t>
   </si>
   <si>
-    <t>0x80244007 エラー</t>
-  </si>
-  <si>
     <t xml:space="preserve"> エラーの Windows</t>
-  </si>
-  <si>
-    <t>デスクトップ画面の左下にある「スタート」ボタンを右クリックし、メニューから「Windows PowerShell(管理者)(A)」をクリックする</t>
-  </si>
-  <si>
-    <t>「管理者：Windows PowerShell」と表示されているウィンドウが開いたことを確認する</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">PowerShellウィンドウに </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>Start-Transcript</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="游ゴシック"/>
-        <family val="2"/>
-        <charset val="128"/>
-      </rPr>
-      <t xml:space="preserve"> と入力し、[Enter]キーを押す</t>
-    </r>
   </si>
   <si>
     <r>
@@ -202,16 +152,108 @@
     </r>
   </si>
   <si>
-    <t>Windowsの設定画面に戻り、「更新とセキュリティ」→「Windows Update」にアクセスする</t>
-  </si>
-  <si>
     <t>「更新プログラムのチェック」ボタンをクリックする</t>
   </si>
   <si>
-    <t>正常に更新がチェックする</t>
-  </si>
-  <si>
     <t>Powershell-Windows</t>
+  </si>
+  <si>
+    <t>メニューから「設定」アイコンをクリックする</t>
+  </si>
+  <si>
+    <t>左側のメニューからWindows Updateをクリックし、Windows Update画面に移動する</t>
+  </si>
+  <si>
+    <t>bdot20240415_141954/1.png</t>
+  </si>
+  <si>
+    <t>bdot20240415_141954/2.png</t>
+  </si>
+  <si>
+    <t>bdot20240415_141954/3.png</t>
+  </si>
+  <si>
+    <t>デスクトップ画面の左下にある「スタート」ボタンを右クリックする</t>
+  </si>
+  <si>
+    <r>
+      <t>メニューからターミナル</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(管理者)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>をクリックする</t>
+    </r>
+  </si>
+  <si>
+    <t>ユーザーアカウント制御と表示されているウィンドウが開いたことを確認する</t>
+  </si>
+  <si>
+    <r>
+      <t>PowerShellウィンドウに s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>tart-transcript</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve"> と入力し、[Enter]キーを押す</t>
+    </r>
+  </si>
+  <si>
+    <t>「スタート」ボタンをクリックする</t>
+  </si>
+  <si>
+    <t>bdot20240415_141954/4.png</t>
+  </si>
+  <si>
+    <t>bdot20240415_141954/5.png</t>
+  </si>
+  <si>
+    <t>bdot20240415_141954/6.png</t>
+  </si>
+  <si>
+    <t>bdot20240415_141954/7.png</t>
+  </si>
+  <si>
+    <t>bdot20240415_141954/8.png</t>
+  </si>
+  <si>
+    <t>bdot20240415_141954/9.png</t>
+  </si>
+  <si>
+    <t>bdot20240415_141954/10.png</t>
+  </si>
+  <si>
+    <t>bdot20240415_141954/11.png</t>
+  </si>
+  <si>
+    <t>0x80240fff エラー</t>
   </si>
 </sst>
 </file>
@@ -222,7 +264,7 @@
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ h:mm"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -278,6 +320,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -697,7 +745,7 @@
   <dimension ref="A1:AD32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3984375" defaultRowHeight="18"/>
@@ -791,7 +839,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>18</v>
@@ -806,10 +854,10 @@
         <v>16</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:30">
@@ -826,7 +874,7 @@
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>19</v>
@@ -841,10 +889,10 @@
         <v>16</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="K3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -861,7 +909,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>19</v>
@@ -876,10 +924,10 @@
         <v>16</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="K4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -887,7 +935,7 @@
         <v>45395.597268518497</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>13</v>
@@ -896,7 +944,7 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>19</v>
@@ -911,10 +959,16 @@
         <v>16</v>
       </c>
       <c r="J5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" t="s">
         <v>22</v>
-      </c>
-      <c r="K5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:30">
@@ -931,7 +985,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>19</v>
@@ -946,10 +1000,10 @@
         <v>16</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:30">
@@ -957,7 +1011,7 @@
         <v>45395.597280092596</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>13</v>
@@ -966,7 +1020,7 @@
         <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>19</v>
@@ -981,16 +1035,10 @@
         <v>16</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="K7" t="s">
-        <v>28</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:30">
@@ -1007,7 +1055,7 @@
         <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>19</v>
@@ -1022,10 +1070,10 @@
         <v>16</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="K8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:30">
@@ -1043,7 +1091,7 @@
         <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>19</v>
@@ -1058,15 +1106,15 @@
         <v>16</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="K9" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:30">
       <c r="A10" s="4">
-        <f t="shared" ref="A10:A16" si="0">A9 + TIME(0, 0, 1)</f>
+        <f t="shared" ref="A10:A12" si="0">A9 + TIME(0, 0, 1)</f>
         <v>45395.597303240756</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1079,7 +1127,7 @@
         <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>19</v>
@@ -1094,10 +1142,10 @@
         <v>16</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K10" t="s">
-        <v>32</v>
+        <v>42</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -1115,7 +1163,7 @@
         <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>19</v>
@@ -1130,10 +1178,10 @@
         <v>16</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:30">
@@ -1151,7 +1199,7 @@
         <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>19</v>
@@ -1166,15 +1214,15 @@
         <v>16</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="4">
-        <f t="shared" si="0"/>
+        <f>A12 + TIME(0, 0, 1)</f>
         <v>45395.597337962987</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1187,7 +1235,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>19</v>
@@ -1202,15 +1250,15 @@
         <v>16</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="K13" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:30">
       <c r="A14" s="4">
-        <f t="shared" si="0"/>
+        <f>A13 + TIME(0, 0, 1)</f>
         <v>45395.597349537064</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1223,7 +1271,7 @@
         <v>14</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>19</v>
@@ -1238,15 +1286,15 @@
         <v>16</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="K14" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="4">
-        <f t="shared" si="0"/>
+        <f>A14 + TIME(0, 0, 1)</f>
         <v>45395.59736111114</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1259,7 +1307,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>19</v>
@@ -1274,15 +1322,15 @@
         <v>16</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="K15" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:30">
       <c r="A16" s="4">
-        <f t="shared" si="0"/>
+        <f>A15 + TIME(0, 0, 1)</f>
         <v>45395.597372685217</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1295,7 +1343,7 @@
         <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>19</v>
@@ -1310,47 +1358,57 @@
         <v>16</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="K16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="4"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:10">
       <c r="A22" s="4"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:10">
       <c r="A23" s="4"/>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:10">
       <c r="A24" s="4"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:10">
       <c r="A25" s="4"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:10">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:10">
       <c r="A27" s="4"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:10">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:10">
       <c r="A29" s="4"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:10">
       <c r="A30" s="4"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:10">
       <c r="A31" s="4"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:10">
       <c r="A32" s="4"/>
     </row>
   </sheetData>

</xml_diff>